<commit_message>
Hack to default to plot derived prods for now
</commit_message>
<xml_diff>
--- a/README_Sample_Data.xlsx
+++ b/README_Sample_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daurin/GitRepos/HyperCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6421BEC-3510-444A-98C1-82522A880427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ACF65F-82F2-0046-BE8F-19D234F9E5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38160" yWindow="500" windowWidth="42100" windowHeight="13840" xr2:uid="{43498CA6-A785-6C4D-A107-6504C485FA78}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33660" windowHeight="18340" xr2:uid="{43498CA6-A785-6C4D-A107-6504C485FA78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <t>Autonomious 10-minute file.</t>
   </si>
   <si>
-    <t>Autonomous 27-minute file matched in time to TriOS FICE22 stations.</t>
+    <t>Autonomous 27-minute file matched in time to TriOS FICE22 stations. Min/max rotator: -126/+42</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>

</xml_diff>